<commit_message>
Update RDFS and add SHACL
</commit_message>
<xml_diff>
--- a/ApplicationProfiles/Grid_Modelling_Appendix_3_LTDS_Profiles_in_RDFS/Comparisons/Comparison_v1_vs_v1-0-1/EQdiff.xlsx
+++ b/ApplicationProfiles/Grid_Modelling_Appendix_3_LTDS_Profiles_in_RDFS/Comparisons/Comparison_v1_vs_v1-0-1/EQdiff.xlsx
@@ -9,13 +9,13 @@
     <sheet name="RDFS comparison results" r:id="rId3" sheetId="1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'RDFS comparison results'!$A$1:$NO$380</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="true">'RDFS comparison results'!$A$1:$OG$398</definedName>
   </definedNames>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1592" uniqueCount="327">
   <si>
     <t>Item</t>
   </si>
@@ -26,7 +26,7 @@
     <t>Value Model A: LTDS_Merged_EQ_RDFSv2020.rdf</t>
   </si>
   <si>
-    <t>Value Model B: LTDS_Merged_EQ_RDFSv2020_v1-0-1.rdf</t>
+    <t>Value Model B: LTDS_Merged_EQ_RDFSv2020_v1-0-1n.rdf</t>
   </si>
   <si>
     <t>ACDCTerminal</t>
@@ -587,6 +587,30 @@
     <t>IdentifiedObject</t>
   </si>
   <si>
+    <t>IdentifiedObject.energyIdentCodeEic</t>
+  </si>
+  <si>
+    <t>The attribute is used for an exchange of the EIC code (Energy identification Code). The length of the string is 16 characters as defined by the EIC code. For details on EIC scheme please refer to ENTSO-E web site.</t>
+  </si>
+  <si>
+    <t>cim:IdentifiedObject</t>
+  </si>
+  <si>
+    <t>"energyIdentCodeEic"@en</t>
+  </si>
+  <si>
+    <t>deprecated</t>
+  </si>
+  <si>
+    <t>IdentifiedObject.shortName</t>
+  </si>
+  <si>
+    <t>The attribute is used for an exchange of a human readable short name with length of the string 12 characters maximum.</t>
+  </si>
+  <si>
+    <t>"shortName"@en</t>
+  </si>
+  <si>
     <t>Inductance</t>
   </si>
   <si>
@@ -644,7 +668,7 @@
     <t>"2023-06-26"^^xsd:date</t>
   </si>
   <si>
-    <t>"2024-07-18"^^xsd:date</t>
+    <t>"2024-07-25"^^xsd:date</t>
   </si>
   <si>
     <t>OperationalLimit</t>
@@ -1065,7 +1089,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D380"/>
+  <dimension ref="A1:D398"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true">
       <pane ySplit="1.0" state="frozen" topLeftCell="A2" activePane="bottomLeft"/>
@@ -4235,284 +4259,284 @@
         <v>188</v>
       </c>
       <c r="B226" t="s" s="2">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C226" t="s" s="2">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D226" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="B227" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="C227" t="s" s="2">
         <v>189</v>
       </c>
-      <c r="B227" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="C227" t="s" s="2">
-        <v>10</v>
-      </c>
       <c r="D227" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="s" s="2">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B228" t="s" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C228" t="s" s="2">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D228" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="229">
       <c r="A229" t="s" s="2">
+        <v>188</v>
+      </c>
+      <c r="B229" t="s" s="2">
+        <v>34</v>
+      </c>
+      <c r="C229" t="s" s="2">
         <v>190</v>
       </c>
-      <c r="B229" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="C229" t="s" s="2">
-        <v>10</v>
-      </c>
       <c r="D229" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="230">
       <c r="A230" t="s" s="2">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B230" t="s" s="2">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C230" t="s" s="2">
-        <v>24</v>
+        <v>191</v>
       </c>
       <c r="D230" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="231">
       <c r="A231" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B231" t="s" s="2">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C231" t="s" s="2">
-        <v>11</v>
+        <v>53</v>
       </c>
       <c r="D231" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="s" s="2">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B232" t="s" s="2">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C232" t="s" s="2">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="D232" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="233">
       <c r="A233" t="s" s="2">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="B233" t="s" s="2">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C233" t="s" s="2">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D233" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="s" s="2">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="B234" t="s" s="2">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C234" t="s" s="2">
-        <v>6</v>
+        <v>192</v>
       </c>
       <c r="D234" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="s" s="2">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B235" t="s" s="2">
-        <v>5</v>
+        <v>27</v>
       </c>
       <c r="C235" t="s" s="2">
-        <v>6</v>
+        <v>28</v>
       </c>
       <c r="D235" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="236">
       <c r="A236" t="s" s="2">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B236" t="s" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C236" t="s" s="2">
-        <v>6</v>
+        <v>194</v>
       </c>
       <c r="D236" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="237">
       <c r="A237" t="s" s="2">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B237" t="s" s="2">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="C237" t="s" s="2">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="D237" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" t="s" s="2">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="B238" t="s" s="2">
-        <v>5</v>
+        <v>34</v>
       </c>
       <c r="C238" t="s" s="2">
-        <v>6</v>
+        <v>190</v>
       </c>
       <c r="D238" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="s" s="2">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B239" t="s" s="2">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C239" t="s" s="2">
-        <v>21</v>
+        <v>195</v>
       </c>
       <c r="D239" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="s" s="2">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B240" t="s" s="2">
-        <v>5</v>
+        <v>38</v>
       </c>
       <c r="C240" t="s" s="2">
-        <v>6</v>
+        <v>53</v>
       </c>
       <c r="D240" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="241">
       <c r="A241" t="s" s="2">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="B241" t="s" s="2">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C241" t="s" s="2">
-        <v>6</v>
+        <v>41</v>
       </c>
       <c r="D241" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="s" s="2">
-        <v>199</v>
+        <v>193</v>
       </c>
       <c r="B242" t="s" s="2">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C242" t="s" s="2">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="D242" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="s" s="2">
-        <v>200</v>
+        <v>193</v>
       </c>
       <c r="B243" t="s" s="2">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C243" t="s" s="2">
-        <v>6</v>
+        <v>192</v>
       </c>
       <c r="D243" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="244">
       <c r="A244" t="s" s="2">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="B244" t="s" s="2">
-        <v>202</v>
+        <v>5</v>
       </c>
       <c r="C244" t="s" s="2">
-        <v>203</v>
+        <v>6</v>
       </c>
       <c r="D244" t="s" s="2">
-        <v>204</v>
+        <v>7</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="s" s="2">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="B245" t="s" s="2">
-        <v>205</v>
+        <v>5</v>
       </c>
       <c r="C245" t="s" s="2">
-        <v>206</v>
+        <v>10</v>
       </c>
       <c r="D245" t="s" s="2">
-        <v>207</v>
+        <v>7</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="s" s="2">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="B246" t="s" s="2">
         <v>5</v>
@@ -4526,13 +4550,13 @@
     </row>
     <row r="247">
       <c r="A247" t="s" s="2">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="B247" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C247" t="s" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D247" t="s" s="2">
         <v>7</v>
@@ -4540,13 +4564,13 @@
     </row>
     <row r="248">
       <c r="A248" t="s" s="2">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="B248" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C248" t="s" s="2">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="D248" t="s" s="2">
         <v>7</v>
@@ -4554,13 +4578,13 @@
     </row>
     <row r="249">
       <c r="A249" t="s" s="2">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="B249" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C249" t="s" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D249" t="s" s="2">
         <v>7</v>
@@ -4568,13 +4592,13 @@
     </row>
     <row r="250">
       <c r="A250" t="s" s="2">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="B250" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C250" t="s" s="2">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D250" t="s" s="2">
         <v>7</v>
@@ -4582,7 +4606,7 @@
     </row>
     <row r="251">
       <c r="A251" t="s" s="2">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="B251" t="s" s="2">
         <v>5</v>
@@ -4596,13 +4620,13 @@
     </row>
     <row r="252">
       <c r="A252" t="s" s="2">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="B252" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C252" t="s" s="2">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D252" t="s" s="2">
         <v>7</v>
@@ -4610,13 +4634,13 @@
     </row>
     <row r="253">
       <c r="A253" t="s" s="2">
-        <v>213</v>
+        <v>202</v>
       </c>
       <c r="B253" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C253" t="s" s="2">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D253" t="s" s="2">
         <v>7</v>
@@ -4624,517 +4648,517 @@
     </row>
     <row r="254">
       <c r="A254" t="s" s="2">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="B254" t="s" s="2">
-        <v>215</v>
+        <v>5</v>
       </c>
       <c r="C254" t="s" s="2">
-        <v>216</v>
+        <v>6</v>
       </c>
       <c r="D254" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="255">
       <c r="A255" t="s" s="2">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B255" t="s" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C255" t="s" s="2">
-        <v>217</v>
+        <v>24</v>
       </c>
       <c r="D255" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="s" s="2">
-        <v>214</v>
+        <v>204</v>
       </c>
       <c r="B256" t="s" s="2">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C256" t="s" s="2">
-        <v>218</v>
+        <v>6</v>
       </c>
       <c r="D256" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="257">
       <c r="A257" t="s" s="2">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B257" t="s" s="2">
-        <v>215</v>
+        <v>5</v>
       </c>
       <c r="C257" t="s" s="2">
-        <v>220</v>
+        <v>21</v>
       </c>
       <c r="D257" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="s" s="2">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B258" t="s" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C258" t="s" s="2">
-        <v>221</v>
+        <v>6</v>
       </c>
       <c r="D258" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="s" s="2">
-        <v>219</v>
+        <v>206</v>
       </c>
       <c r="B259" t="s" s="2">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C259" t="s" s="2">
-        <v>222</v>
+        <v>6</v>
       </c>
       <c r="D259" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="s" s="2">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B260" t="s" s="2">
-        <v>215</v>
+        <v>5</v>
       </c>
       <c r="C260" t="s" s="2">
-        <v>224</v>
+        <v>6</v>
       </c>
       <c r="D260" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" t="s" s="2">
-        <v>223</v>
+        <v>208</v>
       </c>
       <c r="B261" t="s" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C261" t="s" s="2">
-        <v>225</v>
+        <v>6</v>
       </c>
       <c r="D261" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="s" s="2">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="B262" t="s" s="2">
-        <v>36</v>
+        <v>210</v>
       </c>
       <c r="C262" t="s" s="2">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="D262" t="s" s="2">
-        <v>29</v>
+        <v>212</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="s" s="2">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="B263" t="s" s="2">
+        <v>213</v>
+      </c>
+      <c r="C263" t="s" s="2">
+        <v>214</v>
+      </c>
+      <c r="D263" t="s" s="2">
         <v>215</v>
-      </c>
-      <c r="C263" t="s" s="2">
-        <v>29</v>
-      </c>
-      <c r="D263" t="s" s="2">
-        <v>228</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="s" s="2">
-        <v>227</v>
+        <v>216</v>
       </c>
       <c r="B264" t="s" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C264" t="s" s="2">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D264" t="s" s="2">
-        <v>229</v>
+        <v>7</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="s" s="2">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="B265" t="s" s="2">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C265" t="s" s="2">
-        <v>29</v>
+        <v>6</v>
       </c>
       <c r="D265" t="s" s="2">
-        <v>230</v>
+        <v>7</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="s" s="2">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="B266" t="s" s="2">
-        <v>215</v>
+        <v>5</v>
       </c>
       <c r="C266" t="s" s="2">
-        <v>232</v>
+        <v>21</v>
       </c>
       <c r="D266" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="s" s="2">
-        <v>231</v>
+        <v>218</v>
       </c>
       <c r="B267" t="s" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C267" t="s" s="2">
-        <v>233</v>
+        <v>6</v>
       </c>
       <c r="D267" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="s" s="2">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="B268" t="s" s="2">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C268" t="s" s="2">
-        <v>234</v>
+        <v>21</v>
       </c>
       <c r="D268" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="s" s="2">
-        <v>235</v>
+        <v>219</v>
       </c>
       <c r="B269" t="s" s="2">
-        <v>215</v>
+        <v>5</v>
       </c>
       <c r="C269" t="s" s="2">
-        <v>236</v>
+        <v>6</v>
       </c>
       <c r="D269" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="270">
       <c r="A270" t="s" s="2">
-        <v>235</v>
+        <v>220</v>
       </c>
       <c r="B270" t="s" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C270" t="s" s="2">
-        <v>237</v>
+        <v>21</v>
       </c>
       <c r="D270" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="s" s="2">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="B271" t="s" s="2">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C271" t="s" s="2">
-        <v>238</v>
+        <v>21</v>
       </c>
       <c r="D271" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="s" s="2">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="B272" t="s" s="2">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C272" t="s" s="2">
-        <v>24</v>
+        <v>224</v>
       </c>
       <c r="D272" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="273">
       <c r="A273" t="s" s="2">
-        <v>239</v>
+        <v>222</v>
       </c>
       <c r="B273" t="s" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C273" t="s" s="2">
-        <v>6</v>
+        <v>225</v>
       </c>
       <c r="D273" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="s" s="2">
-        <v>240</v>
+        <v>222</v>
       </c>
       <c r="B274" t="s" s="2">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C274" t="s" s="2">
-        <v>6</v>
+        <v>226</v>
       </c>
       <c r="D274" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="275">
       <c r="A275" t="s" s="2">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="B275" t="s" s="2">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C275" t="s" s="2">
-        <v>6</v>
+        <v>228</v>
       </c>
       <c r="D275" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="s" s="2">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="B276" t="s" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C276" t="s" s="2">
-        <v>6</v>
+        <v>229</v>
       </c>
       <c r="D276" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="277">
       <c r="A277" t="s" s="2">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="B277" t="s" s="2">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C277" t="s" s="2">
-        <v>11</v>
+        <v>230</v>
       </c>
       <c r="D277" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="278">
       <c r="A278" t="s" s="2">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="B278" t="s" s="2">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C278" t="s" s="2">
-        <v>6</v>
+        <v>232</v>
       </c>
       <c r="D278" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="279">
       <c r="A279" t="s" s="2">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="B279" t="s" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C279" t="s" s="2">
-        <v>11</v>
+        <v>233</v>
       </c>
       <c r="D279" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="s" s="2">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="B280" t="s" s="2">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C280" t="s" s="2">
-        <v>6</v>
+        <v>234</v>
       </c>
       <c r="D280" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="s" s="2">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="B281" t="s" s="2">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C281" t="s" s="2">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D281" t="s" s="2">
-        <v>7</v>
+        <v>236</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="s" s="2">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="B282" t="s" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C282" t="s" s="2">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D282" t="s" s="2">
-        <v>7</v>
+        <v>237</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="s" s="2">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="B283" t="s" s="2">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C283" t="s" s="2">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="D283" t="s" s="2">
-        <v>7</v>
+        <v>238</v>
       </c>
     </row>
     <row r="284">
       <c r="A284" t="s" s="2">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="B284" t="s" s="2">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C284" t="s" s="2">
-        <v>6</v>
+        <v>240</v>
       </c>
       <c r="D284" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="s" s="2">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="B285" t="s" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C285" t="s" s="2">
-        <v>6</v>
+        <v>241</v>
       </c>
       <c r="D285" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="286">
       <c r="A286" t="s" s="2">
-        <v>250</v>
+        <v>239</v>
       </c>
       <c r="B286" t="s" s="2">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C286" t="s" s="2">
-        <v>21</v>
+        <v>242</v>
       </c>
       <c r="D286" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="s" s="2">
-        <v>251</v>
+        <v>243</v>
       </c>
       <c r="B287" t="s" s="2">
-        <v>5</v>
+        <v>223</v>
       </c>
       <c r="C287" t="s" s="2">
-        <v>6</v>
+        <v>244</v>
       </c>
       <c r="D287" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="s" s="2">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B288" t="s" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C288" t="s" s="2">
-        <v>21</v>
+        <v>245</v>
       </c>
       <c r="D288" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="289">
       <c r="A289" t="s" s="2">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="B289" t="s" s="2">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C289" t="s" s="2">
-        <v>11</v>
+        <v>246</v>
       </c>
       <c r="D289" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="s" s="2">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="B290" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C290" t="s" s="2">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D290" t="s" s="2">
         <v>7</v>
@@ -5142,7 +5166,7 @@
     </row>
     <row r="291">
       <c r="A291" t="s" s="2">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B291" t="s" s="2">
         <v>5</v>
@@ -5156,13 +5180,13 @@
     </row>
     <row r="292">
       <c r="A292" t="s" s="2">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B292" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C292" t="s" s="2">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D292" t="s" s="2">
         <v>7</v>
@@ -5170,7 +5194,7 @@
     </row>
     <row r="293">
       <c r="A293" t="s" s="2">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="B293" t="s" s="2">
         <v>5</v>
@@ -5184,13 +5208,13 @@
     </row>
     <row r="294">
       <c r="A294" t="s" s="2">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="B294" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C294" t="s" s="2">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D294" t="s" s="2">
         <v>7</v>
@@ -5198,13 +5222,13 @@
     </row>
     <row r="295">
       <c r="A295" t="s" s="2">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="B295" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C295" t="s" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D295" t="s" s="2">
         <v>7</v>
@@ -5212,13 +5236,13 @@
     </row>
     <row r="296">
       <c r="A296" t="s" s="2">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="B296" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C296" t="s" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D296" t="s" s="2">
         <v>7</v>
@@ -5226,13 +5250,13 @@
     </row>
     <row r="297">
       <c r="A297" t="s" s="2">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="B297" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C297" t="s" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D297" t="s" s="2">
         <v>7</v>
@@ -5240,7 +5264,7 @@
     </row>
     <row r="298">
       <c r="A298" t="s" s="2">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="B298" t="s" s="2">
         <v>5</v>
@@ -5254,13 +5278,13 @@
     </row>
     <row r="299">
       <c r="A299" t="s" s="2">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="B299" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C299" t="s" s="2">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D299" t="s" s="2">
         <v>7</v>
@@ -5268,7 +5292,7 @@
     </row>
     <row r="300">
       <c r="A300" t="s" s="2">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="B300" t="s" s="2">
         <v>5</v>
@@ -5282,7 +5306,7 @@
     </row>
     <row r="301">
       <c r="A301" t="s" s="2">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="B301" t="s" s="2">
         <v>5</v>
@@ -5296,7 +5320,7 @@
     </row>
     <row r="302">
       <c r="A302" t="s" s="2">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="B302" t="s" s="2">
         <v>5</v>
@@ -5310,13 +5334,13 @@
     </row>
     <row r="303">
       <c r="A303" t="s" s="2">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="B303" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C303" t="s" s="2">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D303" t="s" s="2">
         <v>7</v>
@@ -5324,13 +5348,13 @@
     </row>
     <row r="304">
       <c r="A304" t="s" s="2">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="B304" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C304" t="s" s="2">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D304" t="s" s="2">
         <v>7</v>
@@ -5338,7 +5362,7 @@
     </row>
     <row r="305">
       <c r="A305" t="s" s="2">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="B305" t="s" s="2">
         <v>5</v>
@@ -5352,13 +5376,13 @@
     </row>
     <row r="306">
       <c r="A306" t="s" s="2">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B306" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C306" t="s" s="2">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D306" t="s" s="2">
         <v>7</v>
@@ -5366,13 +5390,13 @@
     </row>
     <row r="307">
       <c r="A307" t="s" s="2">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="B307" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C307" t="s" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D307" t="s" s="2">
         <v>7</v>
@@ -5380,13 +5404,13 @@
     </row>
     <row r="308">
       <c r="A308" t="s" s="2">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="B308" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C308" t="s" s="2">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D308" t="s" s="2">
         <v>7</v>
@@ -5394,7 +5418,7 @@
     </row>
     <row r="309">
       <c r="A309" t="s" s="2">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="B309" t="s" s="2">
         <v>5</v>
@@ -5408,13 +5432,13 @@
     </row>
     <row r="310">
       <c r="A310" t="s" s="2">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="B310" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C310" t="s" s="2">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D310" t="s" s="2">
         <v>7</v>
@@ -5422,7 +5446,7 @@
     </row>
     <row r="311">
       <c r="A311" t="s" s="2">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="B311" t="s" s="2">
         <v>5</v>
@@ -5436,13 +5460,13 @@
     </row>
     <row r="312">
       <c r="A312" t="s" s="2">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="B312" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C312" t="s" s="2">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D312" t="s" s="2">
         <v>7</v>
@@ -5450,7 +5474,7 @@
     </row>
     <row r="313">
       <c r="A313" t="s" s="2">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B313" t="s" s="2">
         <v>5</v>
@@ -5464,13 +5488,13 @@
     </row>
     <row r="314">
       <c r="A314" t="s" s="2">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B314" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C314" t="s" s="2">
-        <v>21</v>
+        <v>11</v>
       </c>
       <c r="D314" t="s" s="2">
         <v>7</v>
@@ -5478,7 +5502,7 @@
     </row>
     <row r="315">
       <c r="A315" t="s" s="2">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="B315" t="s" s="2">
         <v>5</v>
@@ -5492,7 +5516,7 @@
     </row>
     <row r="316">
       <c r="A316" t="s" s="2">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="B316" t="s" s="2">
         <v>5</v>
@@ -5506,13 +5530,13 @@
     </row>
     <row r="317">
       <c r="A317" t="s" s="2">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="B317" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C317" t="s" s="2">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D317" t="s" s="2">
         <v>7</v>
@@ -5520,7 +5544,7 @@
     </row>
     <row r="318">
       <c r="A318" t="s" s="2">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B318" t="s" s="2">
         <v>5</v>
@@ -5534,7 +5558,7 @@
     </row>
     <row r="319">
       <c r="A319" t="s" s="2">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B319" t="s" s="2">
         <v>5</v>
@@ -5548,7 +5572,7 @@
     </row>
     <row r="320">
       <c r="A320" t="s" s="2">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B320" t="s" s="2">
         <v>5</v>
@@ -5562,13 +5586,13 @@
     </row>
     <row r="321">
       <c r="A321" t="s" s="2">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B321" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C321" t="s" s="2">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D321" t="s" s="2">
         <v>7</v>
@@ -5576,13 +5600,13 @@
     </row>
     <row r="322">
       <c r="A322" t="s" s="2">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="B322" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C322" t="s" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D322" t="s" s="2">
         <v>7</v>
@@ -5590,7 +5614,7 @@
     </row>
     <row r="323">
       <c r="A323" t="s" s="2">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B323" t="s" s="2">
         <v>5</v>
@@ -5604,13 +5628,13 @@
     </row>
     <row r="324">
       <c r="A324" t="s" s="2">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B324" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C324" t="s" s="2">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="D324" t="s" s="2">
         <v>7</v>
@@ -5618,13 +5642,13 @@
     </row>
     <row r="325">
       <c r="A325" t="s" s="2">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B325" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C325" t="s" s="2">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D325" t="s" s="2">
         <v>7</v>
@@ -5632,13 +5656,13 @@
     </row>
     <row r="326">
       <c r="A326" t="s" s="2">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="B326" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C326" t="s" s="2">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D326" t="s" s="2">
         <v>7</v>
@@ -5646,13 +5670,13 @@
     </row>
     <row r="327">
       <c r="A327" t="s" s="2">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B327" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C327" t="s" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D327" t="s" s="2">
         <v>7</v>
@@ -5660,13 +5684,13 @@
     </row>
     <row r="328">
       <c r="A328" t="s" s="2">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="B328" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C328" t="s" s="2">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D328" t="s" s="2">
         <v>7</v>
@@ -5674,13 +5698,13 @@
     </row>
     <row r="329">
       <c r="A329" t="s" s="2">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="B329" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C329" t="s" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D329" t="s" s="2">
         <v>7</v>
@@ -5688,13 +5712,13 @@
     </row>
     <row r="330">
       <c r="A330" t="s" s="2">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="B330" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C330" t="s" s="2">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D330" t="s" s="2">
         <v>7</v>
@@ -5702,7 +5726,7 @@
     </row>
     <row r="331">
       <c r="A331" t="s" s="2">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="B331" t="s" s="2">
         <v>5</v>
@@ -5716,13 +5740,13 @@
     </row>
     <row r="332">
       <c r="A332" t="s" s="2">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="B332" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C332" t="s" s="2">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="D332" t="s" s="2">
         <v>7</v>
@@ -5730,7 +5754,7 @@
     </row>
     <row r="333">
       <c r="A333" t="s" s="2">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="B333" t="s" s="2">
         <v>5</v>
@@ -5744,125 +5768,125 @@
     </row>
     <row r="334">
       <c r="A334" t="s" s="2">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="B334" t="s" s="2">
-        <v>285</v>
+        <v>5</v>
       </c>
       <c r="C334" t="s" s="2">
-        <v>286</v>
+        <v>6</v>
       </c>
       <c r="D334" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="335">
       <c r="A335" t="s" s="2">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B335" t="s" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C335" t="s" s="2">
-        <v>287</v>
+        <v>24</v>
       </c>
       <c r="D335" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="s" s="2">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="B336" t="s" s="2">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C336" t="s" s="2">
-        <v>288</v>
+        <v>6</v>
       </c>
       <c r="D336" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="337">
       <c r="A337" t="s" s="2">
-        <v>284</v>
+        <v>282</v>
       </c>
       <c r="B337" t="s" s="2">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C337" t="s" s="2">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="D337" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="338">
       <c r="A338" t="s" s="2">
-        <v>289</v>
+        <v>283</v>
       </c>
       <c r="B338" t="s" s="2">
-        <v>285</v>
+        <v>5</v>
       </c>
       <c r="C338" t="s" s="2">
-        <v>290</v>
+        <v>6</v>
       </c>
       <c r="D338" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="339">
       <c r="A339" t="s" s="2">
-        <v>289</v>
+        <v>284</v>
       </c>
       <c r="B339" t="s" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C339" t="s" s="2">
-        <v>291</v>
+        <v>6</v>
       </c>
       <c r="D339" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="s" s="2">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B340" t="s" s="2">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C340" t="s" s="2">
-        <v>292</v>
+        <v>11</v>
       </c>
       <c r="D340" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="s" s="2">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B341" t="s" s="2">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C341" t="s" s="2">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="D341" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="s" s="2">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B342" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C342" t="s" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D342" t="s" s="2">
         <v>7</v>
@@ -5870,13 +5894,13 @@
     </row>
     <row r="343">
       <c r="A343" t="s" s="2">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="B343" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C343" t="s" s="2">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D343" t="s" s="2">
         <v>7</v>
@@ -5884,7 +5908,7 @@
     </row>
     <row r="344">
       <c r="A344" t="s" s="2">
-        <v>294</v>
+        <v>286</v>
       </c>
       <c r="B344" t="s" s="2">
         <v>5</v>
@@ -5898,13 +5922,13 @@
     </row>
     <row r="345">
       <c r="A345" t="s" s="2">
-        <v>295</v>
+        <v>287</v>
       </c>
       <c r="B345" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C345" t="s" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D345" t="s" s="2">
         <v>7</v>
@@ -5912,13 +5936,13 @@
     </row>
     <row r="346">
       <c r="A346" t="s" s="2">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="B346" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C346" t="s" s="2">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D346" t="s" s="2">
         <v>7</v>
@@ -5926,13 +5950,13 @@
     </row>
     <row r="347">
       <c r="A347" t="s" s="2">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="B347" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C347" t="s" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D347" t="s" s="2">
         <v>7</v>
@@ -5940,13 +5964,13 @@
     </row>
     <row r="348">
       <c r="A348" t="s" s="2">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="B348" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C348" t="s" s="2">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="D348" t="s" s="2">
         <v>7</v>
@@ -5954,13 +5978,13 @@
     </row>
     <row r="349">
       <c r="A349" t="s" s="2">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="B349" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C349" t="s" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D349" t="s" s="2">
         <v>7</v>
@@ -5968,7 +5992,7 @@
     </row>
     <row r="350">
       <c r="A350" t="s" s="2">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="B350" t="s" s="2">
         <v>5</v>
@@ -5982,13 +6006,13 @@
     </row>
     <row r="351">
       <c r="A351" t="s" s="2">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="B351" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C351" t="s" s="2">
-        <v>21</v>
+        <v>6</v>
       </c>
       <c r="D351" t="s" s="2">
         <v>7</v>
@@ -5996,125 +6020,125 @@
     </row>
     <row r="352">
       <c r="A352" t="s" s="2">
-        <v>300</v>
+        <v>292</v>
       </c>
       <c r="B352" t="s" s="2">
-        <v>5</v>
+        <v>293</v>
       </c>
       <c r="C352" t="s" s="2">
-        <v>6</v>
+        <v>294</v>
       </c>
       <c r="D352" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="353">
       <c r="A353" t="s" s="2">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B353" t="s" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C353" t="s" s="2">
-        <v>21</v>
+        <v>295</v>
       </c>
       <c r="D353" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="354">
       <c r="A354" t="s" s="2">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="B354" t="s" s="2">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C354" t="s" s="2">
-        <v>6</v>
+        <v>296</v>
       </c>
       <c r="D354" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="355">
       <c r="A355" t="s" s="2">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="B355" t="s" s="2">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C355" t="s" s="2">
-        <v>10</v>
+        <v>82</v>
       </c>
       <c r="D355" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="356">
       <c r="A356" t="s" s="2">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B356" t="s" s="2">
-        <v>5</v>
+        <v>293</v>
       </c>
       <c r="C356" t="s" s="2">
-        <v>24</v>
+        <v>298</v>
       </c>
       <c r="D356" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="357">
       <c r="A357" t="s" s="2">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="B357" t="s" s="2">
-        <v>5</v>
+        <v>30</v>
       </c>
       <c r="C357" t="s" s="2">
-        <v>6</v>
+        <v>299</v>
       </c>
       <c r="D357" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="358">
       <c r="A358" t="s" s="2">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B358" t="s" s="2">
-        <v>5</v>
+        <v>36</v>
       </c>
       <c r="C358" t="s" s="2">
-        <v>10</v>
+        <v>300</v>
       </c>
       <c r="D358" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="359">
       <c r="A359" t="s" s="2">
-        <v>303</v>
+        <v>297</v>
       </c>
       <c r="B359" t="s" s="2">
-        <v>5</v>
+        <v>40</v>
       </c>
       <c r="C359" t="s" s="2">
-        <v>24</v>
+        <v>82</v>
       </c>
       <c r="D359" t="s" s="2">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="360">
       <c r="A360" t="s" s="2">
-        <v>303</v>
+        <v>301</v>
       </c>
       <c r="B360" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C360" t="s" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D360" t="s" s="2">
         <v>7</v>
@@ -6122,13 +6146,13 @@
     </row>
     <row r="361">
       <c r="A361" t="s" s="2">
-        <v>304</v>
+        <v>301</v>
       </c>
       <c r="B361" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C361" t="s" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D361" t="s" s="2">
         <v>7</v>
@@ -6136,13 +6160,13 @@
     </row>
     <row r="362">
       <c r="A362" t="s" s="2">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="B362" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C362" t="s" s="2">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D362" t="s" s="2">
         <v>7</v>
@@ -6150,13 +6174,13 @@
     </row>
     <row r="363">
       <c r="A363" t="s" s="2">
-        <v>305</v>
+        <v>303</v>
       </c>
       <c r="B363" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C363" t="s" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D363" t="s" s="2">
         <v>7</v>
@@ -6164,13 +6188,13 @@
     </row>
     <row r="364">
       <c r="A364" t="s" s="2">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B364" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C364" t="s" s="2">
-        <v>24</v>
+        <v>6</v>
       </c>
       <c r="D364" t="s" s="2">
         <v>7</v>
@@ -6198,7 +6222,7 @@
         <v>5</v>
       </c>
       <c r="C366" t="s" s="2">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="D366" t="s" s="2">
         <v>7</v>
@@ -6206,13 +6230,13 @@
     </row>
     <row r="367">
       <c r="A367" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B367" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C367" t="s" s="2">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="D367" t="s" s="2">
         <v>7</v>
@@ -6240,7 +6264,7 @@
         <v>5</v>
       </c>
       <c r="C369" t="s" s="2">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="D369" t="s" s="2">
         <v>7</v>
@@ -6265,13 +6289,13 @@
         <v>309</v>
       </c>
       <c r="B371" t="s" s="2">
-        <v>310</v>
+        <v>5</v>
       </c>
       <c r="C371" t="s" s="2">
-        <v>311</v>
+        <v>21</v>
       </c>
       <c r="D371" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="372">
@@ -6279,108 +6303,108 @@
         <v>309</v>
       </c>
       <c r="B372" t="s" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C372" t="s" s="2">
-        <v>312</v>
+        <v>6</v>
       </c>
       <c r="D372" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="373">
       <c r="A373" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B373" t="s" s="2">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C373" t="s" s="2">
-        <v>313</v>
+        <v>10</v>
       </c>
       <c r="D373" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="374">
       <c r="A374" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B374" t="s" s="2">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C374" t="s" s="2">
-        <v>82</v>
+        <v>24</v>
       </c>
       <c r="D374" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="375">
       <c r="A375" t="s" s="2">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="B375" t="s" s="2">
-        <v>310</v>
+        <v>5</v>
       </c>
       <c r="C375" t="s" s="2">
-        <v>315</v>
+        <v>6</v>
       </c>
       <c r="D375" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="376">
       <c r="A376" t="s" s="2">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B376" t="s" s="2">
-        <v>30</v>
+        <v>5</v>
       </c>
       <c r="C376" t="s" s="2">
-        <v>316</v>
+        <v>10</v>
       </c>
       <c r="D376" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="377">
       <c r="A377" t="s" s="2">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B377" t="s" s="2">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="C377" t="s" s="2">
-        <v>317</v>
+        <v>24</v>
       </c>
       <c r="D377" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="378">
       <c r="A378" t="s" s="2">
-        <v>314</v>
+        <v>311</v>
       </c>
       <c r="B378" t="s" s="2">
-        <v>40</v>
+        <v>5</v>
       </c>
       <c r="C378" t="s" s="2">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="D378" t="s" s="2">
-        <v>29</v>
+        <v>7</v>
       </c>
     </row>
     <row r="379">
       <c r="A379" t="s" s="2">
-        <v>318</v>
+        <v>312</v>
       </c>
       <c r="B379" t="s" s="2">
         <v>5</v>
       </c>
       <c r="C379" t="s" s="2">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D379" t="s" s="2">
         <v>7</v>
@@ -6388,20 +6412,272 @@
     </row>
     <row r="380">
       <c r="A380" t="s" s="2">
+        <v>312</v>
+      </c>
+      <c r="B380" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C380" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="D380" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="381">
+      <c r="A381" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="B381" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C381" t="s" s="2">
+        <v>10</v>
+      </c>
+      <c r="D381" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="382">
+      <c r="A382" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="B382" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C382" t="s" s="2">
+        <v>24</v>
+      </c>
+      <c r="D382" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="383">
+      <c r="A383" t="s" s="2">
+        <v>313</v>
+      </c>
+      <c r="B383" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C383" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D383" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="384">
+      <c r="A384" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="B384" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C384" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="D384" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="385">
+      <c r="A385" t="s" s="2">
+        <v>314</v>
+      </c>
+      <c r="B385" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C385" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D385" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="386">
+      <c r="A386" t="s" s="2">
+        <v>315</v>
+      </c>
+      <c r="B386" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C386" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D386" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="387">
+      <c r="A387" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="B387" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C387" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="D387" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="388">
+      <c r="A388" t="s" s="2">
+        <v>316</v>
+      </c>
+      <c r="B388" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C388" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D388" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="389">
+      <c r="A389" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="B389" t="s" s="2">
         <v>318</v>
       </c>
-      <c r="B380" t="s" s="2">
-        <v>5</v>
-      </c>
-      <c r="C380" t="s" s="2">
-        <v>6</v>
-      </c>
-      <c r="D380" t="s" s="2">
+      <c r="C389" t="s" s="2">
+        <v>319</v>
+      </c>
+      <c r="D389" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="390">
+      <c r="A390" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="B390" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="C390" t="s" s="2">
+        <v>320</v>
+      </c>
+      <c r="D390" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="391">
+      <c r="A391" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="B391" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="C391" t="s" s="2">
+        <v>321</v>
+      </c>
+      <c r="D391" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="392">
+      <c r="A392" t="s" s="2">
+        <v>317</v>
+      </c>
+      <c r="B392" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C392" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="D392" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="393">
+      <c r="A393" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="B393" t="s" s="2">
+        <v>318</v>
+      </c>
+      <c r="C393" t="s" s="2">
+        <v>323</v>
+      </c>
+      <c r="D393" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="394">
+      <c r="A394" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="B394" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="C394" t="s" s="2">
+        <v>324</v>
+      </c>
+      <c r="D394" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="395">
+      <c r="A395" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="B395" t="s" s="2">
+        <v>36</v>
+      </c>
+      <c r="C395" t="s" s="2">
+        <v>325</v>
+      </c>
+      <c r="D395" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="396">
+      <c r="A396" t="s" s="2">
+        <v>322</v>
+      </c>
+      <c r="B396" t="s" s="2">
+        <v>40</v>
+      </c>
+      <c r="C396" t="s" s="2">
+        <v>82</v>
+      </c>
+      <c r="D396" t="s" s="2">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="397">
+      <c r="A397" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="B397" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C397" t="s" s="2">
+        <v>11</v>
+      </c>
+      <c r="D397" t="s" s="2">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="398">
+      <c r="A398" t="s" s="2">
+        <v>326</v>
+      </c>
+      <c r="B398" t="s" s="2">
+        <v>5</v>
+      </c>
+      <c r="C398" t="s" s="2">
+        <v>6</v>
+      </c>
+      <c r="D398" t="s" s="2">
         <v>7</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:NO380"/>
+  <autoFilter ref="A1:OG398"/>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
@@ -6751,13 +7027,13 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CE89CDF-E914-4FE9-924B-9281341C7363}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D4D595D9-D9AF-4A27-B8C2-9550FDA16261}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{690506B7-41E9-4260-80A2-491A401BCA9B}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{95A2EBB1-12E2-4F2C-9B0C-9942EB41DCE9}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8E3D212-342B-4AB6-94AB-86CCA5F137F5}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08C3BF7B-AC0D-4C4A-AD81-653E69069F9F}"/>
 </file>
</xml_diff>